<commit_message>
Add patient characteristics tables related to disease stage and functional status.
</commit_message>
<xml_diff>
--- a/docs/model-doc/tables-raw/patchars.xlsx
+++ b/docs/model-doc/tables-raw/patchars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="80" windowWidth="25040" windowHeight="14020" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="80" windowWidth="25040" windowHeight="14020" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="patchar-1-1L" sheetId="1" r:id="rId1"/>
@@ -227,9 +227,6 @@
     <t>Gefitinib (66%) /Erlotinib (34%)</t>
   </si>
   <si>
-    <t>&lt;1</t>
-  </si>
-  <si>
     <t>histology_adenocarcinoma</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>Yang2014</t>
+  </si>
+  <si>
+    <t>&lt;.01</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -1966,7 +1966,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2943,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3016,7 +3016,7 @@
         <v>0.63</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -3154,40 +3154,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>72</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>74</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>75</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>78</v>
-      </c>
-      <c r="O1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -4120,40 +4120,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>72</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>74</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>75</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>78</v>
-      </c>
-      <c r="O1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:15">

</xml_diff>

<commit_message>
Add treatment characteristics and trial lookup table.
</commit_message>
<xml_diff>
--- a/docs/model-doc/tables-raw/patchars.xlsx
+++ b/docs/model-doc/tables-raw/patchars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="80" windowWidth="25040" windowHeight="14020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="60" yWindow="80" windowWidth="25040" windowHeight="14020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="patchar-1-1L" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="80">
   <si>
     <t>trial_id</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Gefitinib (66%) / Erlotinib (34%)</t>
   </si>
   <si>
-    <t>Han 2017</t>
-  </si>
-  <si>
     <t>Carboplatin + Pemetrexed + Gefitinib</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
   </si>
   <si>
     <t>Docetaxel + Cisplatin</t>
-  </si>
-  <si>
-    <t>Yang 2014</t>
   </si>
   <si>
     <t>Cisplatin + Pemetrexed followed by Gefitinib maintenance</t>
@@ -318,8 +312,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -344,7 +346,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -355,6 +357,10 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -365,6 +371,10 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -696,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1098,13 +1108,13 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12">
         <v>0.625</v>
@@ -1121,13 +1131,13 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13">
         <v>0.57499999999999996</v>
@@ -1144,7 +1154,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1167,7 +1177,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -1199,13 +1209,13 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
       <c r="D16">
         <v>57</v>
@@ -1231,10 +1241,10 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -1248,13 +1258,13 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
       </c>
       <c r="G18">
         <v>0.79800000000000004</v>
@@ -1265,13 +1275,13 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>61.5</v>
@@ -1303,13 +1313,13 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20">
         <v>61</v>
@@ -1341,13 +1351,13 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>58</v>
@@ -1370,7 +1380,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -1399,13 +1409,13 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>63</v>
@@ -1434,7 +1444,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -1469,7 +1479,7 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -1498,13 +1508,13 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26">
         <v>35</v>
@@ -1527,7 +1537,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -1559,13 +1569,13 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28">
         <v>59</v>
@@ -1591,7 +1601,7 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -1620,13 +1630,13 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
         <v>48</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
       </c>
       <c r="D30">
         <v>64</v>
@@ -1649,13 +1659,13 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31">
         <v>59</v>
@@ -1681,7 +1691,7 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -1966,7 +1976,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1982,40 +1992,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>61</v>
-      </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -2029,7 +2039,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <v>0.33</v>
@@ -2055,7 +2065,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>0.28000000000000003</v>
@@ -2081,7 +2091,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>0.14699999999999999</v>
@@ -2110,7 +2120,7 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5">
         <v>0.14399999999999999</v>
@@ -2139,7 +2149,7 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6">
         <v>0.31</v>
@@ -2171,7 +2181,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7">
         <v>0.34</v>
@@ -2203,7 +2213,7 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8">
         <v>0.25800000000000001</v>
@@ -2232,7 +2242,7 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9">
         <v>0.20699999999999999</v>
@@ -2261,7 +2271,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10">
         <v>0.4</v>
@@ -2287,10 +2297,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>0.42</v>
@@ -2310,16 +2320,16 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12">
         <v>0.2</v>
@@ -2339,16 +2349,16 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E13">
         <v>0.25</v>
@@ -2368,7 +2378,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -2377,7 +2387,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14">
         <v>0.22</v>
@@ -2397,7 +2407,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -2406,7 +2416,7 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15">
         <v>0.25800000000000001</v>
@@ -2441,16 +2451,16 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16">
         <v>0.26500000000000001</v>
@@ -2485,16 +2495,16 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G17">
         <v>0.90200000000000002</v>
@@ -2502,16 +2512,16 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G18">
         <v>0.94599999999999995</v>
@@ -2519,16 +2529,16 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19">
         <v>0.4</v>
@@ -2548,16 +2558,16 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E20">
         <v>0.35699999999999998</v>
@@ -2577,16 +2587,16 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E21">
         <v>0.19800000000000001</v>
@@ -2609,7 +2619,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -2618,7 +2628,7 @@
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E22">
         <v>0.33600000000000002</v>
@@ -2641,16 +2651,16 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23">
         <v>0.32</v>
@@ -2673,7 +2683,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -2682,7 +2692,7 @@
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E24">
         <v>0.3</v>
@@ -2705,7 +2715,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -2714,7 +2724,7 @@
         <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E25">
         <v>0.47399999999999998</v>
@@ -2734,16 +2744,16 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E26">
         <v>0.5</v>
@@ -2763,7 +2773,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -2772,7 +2782,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G27">
         <v>0.91</v>
@@ -2789,16 +2799,16 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G28">
         <v>0.96</v>
@@ -2815,7 +2825,7 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -2824,7 +2834,7 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E29">
         <v>0.65100000000000002</v>
@@ -2844,16 +2854,16 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E30">
         <v>0.60499999999999998</v>
@@ -2873,16 +2883,16 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E31">
         <v>0.42</v>
@@ -2902,7 +2912,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -2911,7 +2921,7 @@
         <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E32">
         <v>0.42</v>
@@ -2931,6 +2941,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2943,7 +2954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2960,40 +2971,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>61</v>
-      </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3007,7 +3018,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E2">
         <v>0.37</v>
@@ -3016,7 +3027,7 @@
         <v>0.63</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -3030,7 +3041,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>0.37</v>
@@ -3056,7 +3067,7 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <v>0.4</v>
@@ -3082,7 +3093,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>0.41</v>
@@ -3108,7 +3119,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6">
         <v>0.4</v>
@@ -3137,8 +3148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3154,40 +3165,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>76</v>
-      </c>
-      <c r="N1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3465,7 +3476,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11">
         <v>0.98</v>
@@ -3488,13 +3499,13 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3511,13 +3522,13 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3534,7 +3545,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -3557,7 +3568,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -3592,13 +3603,13 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
       <c r="D16">
         <v>0.97199999999999998</v>
@@ -3627,10 +3638,10 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -3641,13 +3652,13 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -3655,13 +3666,13 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -3684,13 +3695,13 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3713,13 +3724,13 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -3742,7 +3753,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -3771,13 +3782,13 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>0.99</v>
@@ -3797,7 +3808,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -3823,7 +3834,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -3861,13 +3872,13 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26">
         <v>0.96499999999999997</v>
@@ -3899,7 +3910,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -3928,13 +3939,13 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28">
         <v>0.86</v>
@@ -3957,7 +3968,7 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -3986,13 +3997,13 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
         <v>48</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -4015,13 +4026,13 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31">
         <v>0.97</v>
@@ -4053,7 +4064,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -4091,6 +4102,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4120,40 +4132,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>76</v>
-      </c>
-      <c r="N1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:15">

</xml_diff>